<commit_message>
Fix: Ta certo agora confia
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -533,22 +533,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>19.440.696/0001-03</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Não Disponível</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Fabio Modesto, 158</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vila Joaquim Sales</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -595,22 +595,22 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>09.371.163/0001-55</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>LABOMINAS</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua A, Alphaville Ii</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Coqueiro</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -657,22 +657,22 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>09.371.163/0001-55</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>LABOMINAS</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua A, Alphaville Ii</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Coqueiro</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -719,27 +719,27 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>05.642.544/0001-70</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Não Disponível</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Uruguai, 533</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>85.805-010</t>
         </is>
       </c>
     </row>
@@ -781,27 +781,27 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>05.642.544/0001-70</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Não Disponível</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Uruguai, 533</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Centro</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>85.805-010</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>13.280.276/0001-12</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>46.139.952/0001-91</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -977,17 +977,17 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Padre Joao, 11-25</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vila Santa Tereza</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>17.012-020</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>46.139.952/0001-91</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1039,17 +1039,17 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Padre Joao, 11-25</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vila Santa Tereza</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>17.012-020</t>
         </is>
       </c>
     </row>
@@ -1091,27 +1091,27 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>61.486.650/0001-83</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Não Disponível</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Avenida Jurua, 434</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Alphaville Centro Industrial e Empresarial/alphaville.</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>06.455-010</t>
         </is>
       </c>
     </row>
@@ -1153,27 +1153,27 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>60.160.546/0001-31</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>DIGIMED</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua dos Marianos, 227</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vila Gea</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>04.691-110</t>
         </is>
       </c>
     </row>
@@ -1215,27 +1215,27 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>60.160.546/0001-31</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>DIGIMED</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua dos Marianos, 227</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Vila Gea</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>04.691-110</t>
         </is>
       </c>
     </row>
@@ -1277,27 +1277,27 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>57.442.774/0001-90</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Não Disponível</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Pedro Stancato, 860</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Chacaras Campos dos Amarais</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>13.082-050</t>
         </is>
       </c>
     </row>
@@ -1401,27 +1401,27 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>33.435.231/0001-87</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>GE CELMA</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Alice Herve, 356</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Bingen</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>25.665-010</t>
         </is>
       </c>
     </row>
@@ -1463,27 +1463,27 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>33.435.231/0001-87</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>GE CELMA</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Alice Herve, 356</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Bingen</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>25.665-010</t>
         </is>
       </c>
     </row>
@@ -1525,27 +1525,27 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>33.435.231/0001-87</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>GE CELMA</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Logradouro:Rua Alice Herve, 356</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Bingen</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>25.665-010</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Feat: Função cache com resultados anteriores
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCCCC"/>
+        <bgColor rgb="00FFCCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -551,7 +558,7 @@
           <t>Vila Joaquim Sales</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -578,12 +585,12 @@
           <t>MANHUACU</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -613,7 +620,7 @@
           <t>Coqueiro</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -675,7 +682,7 @@
           <t>Coqueiro</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -841,27 +848,27 @@
           <t>DEF</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -893,7 +900,7 @@
           <t>PERKINELMER</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -908,22 +915,22 @@
           <t>13.280.276/0001-12</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -970,7 +977,7 @@
           <t>46.139.952/0001-91</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1032,7 +1039,7 @@
           <t>46.139.952/0001-91</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1074,12 +1081,12 @@
           <t>DUQUE DE CAXIAS</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1337,27 +1344,27 @@
           <t>GHI</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
+      <c r="H15" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I15" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>